<commit_message>
Data Transformation and Modeling
</commit_message>
<xml_diff>
--- a/IntermediateData/Features_Analysis.xlsx
+++ b/IntermediateData/Features_Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azimedemtsvd\Dropbox\Tesi Magistrale\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azimedemtsvd\Documents\EnergyField-ChurnPrediction\IntermediateData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2808" uniqueCount="1053">
   <si>
     <t>idn_servizio_sk</t>
   </si>
@@ -2593,12 +2593,6 @@
     <t>Province of supply</t>
   </si>
   <si>
-    <t>Region of supply (ABRUZZO, BASILICATA, LAZIO, EMILIA ROMAGNA, …)</t>
-  </si>
-  <si>
-    <t>Billing region</t>
-  </si>
-  <si>
     <t>Billing geographical location (CENTRO, NORD EST, NORD OVEST, SUD)</t>
   </si>
   <si>
@@ -2627,9 +2621,6 @@
   </si>
   <si>
     <t>1, 0</t>
-  </si>
-  <si>
-    <t>Sub channel (VYBITA SRLS, PUNTO ENEL CUNEO, VISONE GIUSEPPE, …)</t>
   </si>
   <si>
     <t>Virtual assistant (CAT0, CAT1, CAT2)</t>
@@ -2667,35 +2658,6 @@
     <t>Indicates if the client left ENEL 3 months after t0</t>
   </si>
   <si>
-    <t>Client city (CERVETERI, GIARRE, ALBETTONE, VOLVERA, …)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Information already in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sds_provincia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Land type (RURAL, URBAN, METRO)</t>
   </si>
   <si>
@@ -2706,12 +2668,6 @@
   </si>
   <si>
     <t>High NA percentage (91%)</t>
-  </si>
-  <si>
-    <t>Istat</t>
-  </si>
-  <si>
-    <t>Region Id</t>
   </si>
   <si>
     <t>Electric Custers (A &lt;4 kW, B 4&lt;=kW&lt;12, C 12&lt;=kW&lt;25, D 25&lt;=kW&lt;50, E 50&lt;=kW&lt;100, F 100&lt;=kW&lt;200, G 200&lt;=kW&lt;400, H &gt;=400 kW)</t>
@@ -2785,9 +2741,6 @@
   </si>
   <si>
     <t>Indicates if the web bill is active</t>
-  </si>
-  <si>
-    <t>Indicates whether or not the web bill is active</t>
   </si>
   <si>
     <t>Last bill cluster (CICLO, ADJ_STORNO, OTHER)</t>
@@ -3303,9 +3256,6 @@
     <t>This is a technical column</t>
   </si>
   <si>
-    <t>(36+, 24-36, 12-24, 0-12)</t>
-  </si>
-  <si>
     <t>High NA percentage (100%)</t>
   </si>
   <si>
@@ -3476,6 +3426,332 @@
   </si>
   <si>
     <t>Mode (try to compute the mode including the class of the paticular observation)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Contains same information as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_commodity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>One hot (6 columns)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk)</t>
+  </si>
+  <si>
+    <t>Flag (1 for 'SI' and 0 for 'NO')</t>
+  </si>
+  <si>
+    <t>WOE (Weight Of Evidence)</t>
+  </si>
+  <si>
+    <t>Region of supply</t>
+  </si>
+  <si>
+    <t>Billing region (ABRUZZO, BASILICATA, LAZIO, EMILIA ROMAGNA, …)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Calculated the same way as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_provincia_fatturazione</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (bds.T_BDS_ANX_DT_AA_SERVIZI.sds_provincia). Thus is is redundant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Calculated the same way as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_regione_fatturazione</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (bds.T_BDS_ANX_DT_AA_SERVIZI.sds_regione). Thus is is redundant</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Calculated the same way as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_mat_fatturazione</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (bds.T_BDS_ANX_DT_AA_SERVIZI.sds_macro_area_territoriale). Thus is is redundant</t>
+    </r>
+  </si>
+  <si>
+    <t>Flag (1 for 'WB' and 0 for 'NO-WB')</t>
+  </si>
+  <si>
+    <t>Sub channel that acquired the client (VYBITA SRLS, PUNTO ENEL CUNEO, VISONE GIUSEPPE, …)</t>
+  </si>
+  <si>
+    <t>Service city (CERVETERI, GIARRE, ALBETTONE, VOLVERA, …)</t>
+  </si>
+  <si>
+    <t>Service province</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Information already in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_provincia_fatturazione</t>
+    </r>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (servizi.lds_comune)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (servizi.mds_sottocanale)</t>
+  </si>
+  <si>
+    <t>Service Istat code</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (geomarketing_istat.cdc_istat)</t>
+  </si>
+  <si>
+    <t>Istat Id of the billing Region</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Contains same information as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_regione_fatturazione</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>One hot (5 columns)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (EMILIA-ROMAGNA =  EMILIA ROMAGNA and TRENTINO ALTO ADIGE = TRENTINO-ALTO ADIGE)</t>
+  </si>
+  <si>
+    <t>Replace '***' with '-1' and cast as double</t>
+  </si>
+  <si>
+    <t>Altimetric area (1, 2, 3, 4, 5, ***)</t>
+  </si>
+  <si>
+    <t>Istat Metric (T -&gt; Totalmente Montano, P -&gt; Parzialmente Montano, NM -&gt; Non Montano, *** -&gt; NA</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: Replace '***' with -1, 'NM' with 0, 'P' with 1 and 'T' with 2</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: integers from 1 to 8</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: integers from 1 to 7 (with 'ESCLUDI' as 1 and 'F' as 7)</t>
+  </si>
+  <si>
+    <t>Segment Cluster</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Information already in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_cluster_ele</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sds_cluster_gas</t>
+    </r>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (servizi.cdc_causale_attivazione)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Same information as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lds_comune_fornitura</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Indicates whether or not the web bill is active (SI, NO)</t>
+  </si>
+  <si>
+    <t>One hot (3 columns)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (marketing.mds_nome_campagna)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (marketing.xds_canale)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (marketing.xds_tipologia_azione)</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: RESIDENZIALE-&gt;0, MICRO-&gt;1, SMALL-&gt;2, MEDIUM-&gt;3</t>
+  </si>
+  <si>
+    <t>Clusters representing the months invertal in which the service age falls (36+, 24-36, 12-24, 0-12)</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: 0-12-&gt;1, 12-24-&gt;2, 24-36-&gt;3, 36+-&gt;4</t>
+  </si>
+  <si>
+    <t>Clusters representing the months invertal in which the maximum service age of the curent client falls (36+, 24-36, 12-24, 0-12)</t>
+  </si>
+  <si>
+    <t>Ordinal Encoding: negativo-&gt;-1, basso-&gt;0, medio-&gt;1, alto-&gt;2, molto-alto-&gt;3</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (servizi.lds_prodotto_listino_2)</t>
+  </si>
+  <si>
+    <t>Word Embedding (Context Clients: idn_cliente_sk) (servizi.mds_canale_acquisizione)</t>
+  </si>
+  <si>
+    <t>High number of distint values</t>
   </si>
 </sst>
 </file>
@@ -3867,7 +4143,7 @@
   <dimension ref="A1:K768"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3875,8 +4151,8 @@
     <col min="1" max="1" width="99" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="201.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="122.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
@@ -3890,16 +4166,16 @@
         <v>767</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>771</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1000</v>
+        <v>991</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>1013</v>
+        <v>1004</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>768</v>
@@ -3914,10 +4190,10 @@
         <v>776</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>997</v>
+        <v>988</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>998</v>
+        <v>989</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
@@ -3951,7 +4227,7 @@
         <v>788</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3995,9 +4271,11 @@
         <v>774</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>1005</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1027</v>
+      </c>
       <c r="F4" s="1">
         <v>6</v>
       </c>
@@ -4123,9 +4401,11 @@
         <v>774</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>992</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1050</v>
+      </c>
       <c r="F8" s="1">
         <v>220</v>
       </c>
@@ -4173,7 +4453,7 @@
         <v>788</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>978</v>
+        <v>970</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4219,7 +4499,7 @@
         <v>774</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1">
@@ -4239,7 +4519,7 @@
         <v>788</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1008</v>
+        <v>999</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4253,7 +4533,7 @@
         <v>774</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1001</v>
+        <v>992</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1">
@@ -4273,7 +4553,7 @@
         <v>788</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1009</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4351,9 +4631,11 @@
         <v>774</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1010</v>
+      </c>
       <c r="F15" s="1">
         <v>2145479</v>
       </c>
@@ -4368,9 +4650,11 @@
         <v>4.5778157325005002E-2</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1052</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -4430,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="K17" s="1"/>
     </row>
@@ -4445,9 +4729,11 @@
         <v>774</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E18" s="2"/>
+        <v>992</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1051</v>
+      </c>
       <c r="F18" s="1">
         <v>14</v>
       </c>
@@ -4509,9 +4795,11 @@
         <v>774</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E20" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="F20" s="1">
         <v>4736</v>
       </c>
@@ -4559,7 +4847,7 @@
         <v>788</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>1010</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4573,9 +4861,11 @@
         <v>774</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E22" s="2"/>
+        <v>992</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="F22" s="1">
         <v>14</v>
       </c>
@@ -4703,7 +4993,9 @@
       <c r="D26" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>1009</v>
+      </c>
       <c r="F26" s="1">
         <v>2</v>
       </c>
@@ -4753,7 +5045,7 @@
         <v>788</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1012</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4819,7 +5111,7 @@
         <v>787</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>1011</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4869,7 +5161,9 @@
       <c r="D31" s="2" t="s">
         <v>817</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>1007</v>
+      </c>
       <c r="F31" s="1">
         <v>6</v>
       </c>
@@ -4899,9 +5193,11 @@
         <v>774</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E32" s="2"/>
+        <v>992</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>1007</v>
+      </c>
       <c r="F32" s="1">
         <v>6</v>
       </c>
@@ -4965,9 +5261,11 @@
         <v>774</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="F34" s="1">
         <v>108</v>
       </c>
@@ -4997,7 +5295,7 @@
         <v>774</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="1">
@@ -5014,22 +5312,24 @@
         <v>4.7476046974082114E-2</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K35" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>1013</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>824</v>
+        <v>1011</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1">
@@ -5046,26 +5346,30 @@
         <v>4.7476046974082114E-2</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K36" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>1014</v>
+      </c>
     </row>
     <row r="37" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>825</v>
+        <v>1012</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="1">
-        <v>23</v>
+        <v>993</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>1028</v>
       </c>
       <c r="G37" s="1">
         <v>12443</v>
@@ -5087,15 +5391,17 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E38" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>1027</v>
+      </c>
       <c r="F38" s="1">
         <v>5</v>
       </c>
@@ -5119,13 +5425,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="1">
@@ -5142,24 +5448,28 @@
         <v>4.7476046974082114E-2</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K39" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>1015</v>
+      </c>
     </row>
     <row r="40" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E40" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="F40" s="1">
         <v>109</v>
       </c>
@@ -5183,15 +5493,17 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E41" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>1029</v>
+      </c>
       <c r="F41" s="1">
         <v>23</v>
       </c>
@@ -5215,15 +5527,17 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E42" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>1027</v>
+      </c>
       <c r="F42" s="1">
         <v>6</v>
       </c>
@@ -5247,7 +5561,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>774</v>
@@ -5279,7 +5593,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>873</v>
+        <v>865</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>773</v>
@@ -5309,7 +5623,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>773</v>
@@ -5339,7 +5653,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>773</v>
@@ -5369,7 +5683,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>773</v>
@@ -5399,7 +5713,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>874</v>
+        <v>866</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>773</v>
@@ -5429,7 +5743,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>773</v>
@@ -5459,7 +5773,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>773</v>
@@ -5489,7 +5803,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>773</v>
@@ -5519,7 +5833,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>773</v>
@@ -5549,7 +5863,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>773</v>
@@ -5579,7 +5893,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>773</v>
@@ -5609,7 +5923,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>773</v>
@@ -5639,7 +5953,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>773</v>
@@ -5669,7 +5983,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>773</v>
@@ -5699,7 +6013,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>773</v>
@@ -5729,13 +6043,15 @@
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="F59" s="1">
         <v>4</v>
       </c>
@@ -5759,7 +6075,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>773</v>
@@ -5789,13 +6105,15 @@
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>1016</v>
+      </c>
       <c r="F61" s="1">
         <v>2</v>
       </c>
@@ -5819,7 +6137,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>773</v>
@@ -5849,15 +6167,17 @@
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>836</v>
+        <v>1017</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E63" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>1022</v>
+      </c>
       <c r="F63" s="1">
         <v>5371</v>
       </c>
@@ -5881,7 +6201,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>774</v>
@@ -5905,7 +6225,7 @@
         <v>788</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5913,7 +6233,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>773</v>
@@ -5943,7 +6263,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>773</v>
@@ -5973,7 +6293,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>773</v>
@@ -6003,7 +6323,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>773</v>
@@ -6033,7 +6353,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>773</v>
@@ -6063,7 +6383,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>773</v>
@@ -6087,7 +6407,7 @@
         <v>788</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="71" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6095,7 +6415,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>773</v>
@@ -6119,7 +6439,7 @@
         <v>788</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6127,7 +6447,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>773</v>
@@ -6151,7 +6471,7 @@
         <v>788</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="73" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6159,7 +6479,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>773</v>
@@ -6183,7 +6503,7 @@
         <v>788</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="74" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6191,7 +6511,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>773</v>
@@ -6215,7 +6535,7 @@
         <v>788</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -6223,7 +6543,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>773</v>
@@ -6253,7 +6573,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>773</v>
@@ -6283,7 +6603,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>773</v>
@@ -6313,7 +6633,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>773</v>
@@ -6343,7 +6663,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>773</v>
@@ -6373,7 +6693,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>773</v>
@@ -6403,7 +6723,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>773</v>
@@ -6713,7 +7033,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>773</v>
@@ -6743,7 +7063,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>773</v>
@@ -6969,13 +7289,13 @@
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>841</v>
+        <v>1018</v>
       </c>
       <c r="C101" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="1">
@@ -6992,15 +7312,19 @@
         <v>5.2819324777139585</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K101" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>1039</v>
+      </c>
     </row>
     <row r="102" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>1019</v>
+      </c>
       <c r="C102" s="2" t="s">
         <v>774</v>
       </c>
@@ -7023,7 +7347,7 @@
         <v>788</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>842</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="103" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7031,7 +7355,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>774</v>
@@ -7055,7 +7379,7 @@
         <v>788</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="104" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7085,7 +7409,7 @@
         <v>788</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="105" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7093,15 +7417,17 @@
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>847</v>
+        <v>1023</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E105" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>1024</v>
+      </c>
       <c r="F105" s="1">
         <v>7987</v>
       </c>
@@ -7125,13 +7451,13 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>848</v>
+        <v>1025</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>1002</v>
+        <v>993</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="1">
@@ -7148,22 +7474,28 @@
         <v>5.4969654324166284E-2</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K106" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>1026</v>
+      </c>
     </row>
     <row r="107" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B107" s="1"/>
+      <c r="B107" s="1" t="s">
+        <v>1031</v>
+      </c>
       <c r="C107" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E107" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>1030</v>
+      </c>
       <c r="F107" s="1">
         <v>6</v>
       </c>
@@ -7244,14 +7576,18 @@
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="B110" s="1" t="s">
+        <v>1032</v>
+      </c>
       <c r="C110" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E110" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>1033</v>
+      </c>
       <c r="F110" s="1">
         <v>4</v>
       </c>
@@ -7335,13 +7671,15 @@
         <v>111</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
+      <c r="E113" s="2" t="s">
+        <v>1034</v>
+      </c>
       <c r="F113" s="1">
         <v>8</v>
       </c>
@@ -7365,13 +7703,15 @@
         <v>112</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
+      <c r="E114" s="2" t="s">
+        <v>1035</v>
+      </c>
       <c r="F114" s="1">
         <v>7</v>
       </c>
@@ -7394,7 +7734,9 @@
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B115" s="1"/>
+      <c r="B115" s="1" t="s">
+        <v>1036</v>
+      </c>
       <c r="C115" s="2" t="s">
         <v>774</v>
       </c>
@@ -7414,16 +7756,18 @@
         <v>0</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K115" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>1037</v>
+      </c>
     </row>
     <row r="116" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>773</v>
@@ -7449,7 +7793,7 @@
         <v>787</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7457,7 +7801,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>773</v>
@@ -7483,7 +7827,7 @@
         <v>787</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="118" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7491,7 +7835,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>773</v>
@@ -7517,7 +7861,7 @@
         <v>787</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="119" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7549,7 +7893,7 @@
         <v>788</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
     </row>
     <row r="120" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7557,7 +7901,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>774</v>
@@ -7581,7 +7925,7 @@
         <v>788</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
     </row>
     <row r="121" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -7589,15 +7933,17 @@
         <v>119</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E121" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>1038</v>
+      </c>
       <c r="F121" s="1">
         <v>16</v>
       </c>
@@ -7621,7 +7967,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>773</v>
@@ -7651,7 +7997,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>773</v>
@@ -7681,7 +8027,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>773</v>
@@ -7711,7 +8057,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>773</v>
@@ -7741,7 +8087,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>773</v>
@@ -7771,7 +8117,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>773</v>
@@ -7801,7 +8147,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>773</v>
@@ -7831,7 +8177,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>773</v>
@@ -7861,7 +8207,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>773</v>
@@ -7891,7 +8237,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>773</v>
@@ -7921,7 +8267,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>773</v>
@@ -7951,7 +8297,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>773</v>
@@ -7981,7 +8327,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>773</v>
@@ -8011,7 +8357,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>773</v>
@@ -8041,7 +8387,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>773</v>
@@ -8071,7 +8417,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>773</v>
@@ -8101,7 +8447,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>912</v>
+        <v>904</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>773</v>
@@ -8131,7 +8477,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>913</v>
+        <v>905</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>773</v>
@@ -8161,7 +8507,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>773</v>
@@ -8191,7 +8537,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>773</v>
@@ -8221,7 +8567,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>773</v>
@@ -8242,16 +8588,18 @@
         <v>0</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K142" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="143" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>773</v>
@@ -8272,16 +8620,18 @@
         <v>0</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K143" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="144" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>773</v>
@@ -8302,16 +8652,18 @@
         <v>0</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K144" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="145" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>773</v>
@@ -8332,16 +8684,18 @@
         <v>0</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K145" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="146" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>773</v>
@@ -8371,7 +8725,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>773</v>
@@ -8401,7 +8755,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>773</v>
@@ -8431,7 +8785,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>923</v>
+        <v>915</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>773</v>
@@ -8461,7 +8815,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>773</v>
@@ -8491,7 +8845,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>773</v>
@@ -8521,7 +8875,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>773</v>
@@ -8551,7 +8905,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>773</v>
@@ -8581,7 +8935,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>773</v>
@@ -8611,7 +8965,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>773</v>
@@ -8641,7 +8995,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>773</v>
@@ -8671,7 +9025,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>773</v>
@@ -8701,7 +9055,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>773</v>
@@ -8731,7 +9085,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>773</v>
@@ -8761,7 +9115,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>773</v>
@@ -8791,7 +9145,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>773</v>
@@ -8821,7 +9175,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>774</v>
@@ -8845,7 +9199,7 @@
         <v>788</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
     </row>
     <row r="163" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -8853,7 +9207,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>773</v>
@@ -8883,7 +9237,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>773</v>
@@ -8913,7 +9267,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>773</v>
@@ -8943,7 +9297,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>773</v>
@@ -8973,7 +9327,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>773</v>
@@ -9003,7 +9357,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>773</v>
@@ -9033,7 +9387,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>773</v>
@@ -9063,7 +9417,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>773</v>
@@ -9093,7 +9447,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>773</v>
@@ -9123,7 +9477,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>773</v>
@@ -9153,7 +9507,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>773</v>
@@ -9183,7 +9537,7 @@
         <v>172</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>773</v>
@@ -9213,7 +9567,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>773</v>
@@ -9243,7 +9597,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>773</v>
@@ -9273,7 +9627,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>773</v>
@@ -9303,7 +9657,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>773</v>
@@ -9327,7 +9681,7 @@
         <v>787</v>
       </c>
       <c r="K178" s="1" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
     </row>
     <row r="179" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -9335,15 +9689,17 @@
         <v>177</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E179" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>1021</v>
+      </c>
       <c r="F179" s="1">
         <v>7972</v>
       </c>
@@ -9367,13 +9723,15 @@
         <v>178</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>858</v>
+        <v>1040</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D180" s="2"/>
-      <c r="E180" s="2"/>
+      <c r="E180" s="2" t="s">
+        <v>1009</v>
+      </c>
       <c r="F180" s="1">
         <v>2</v>
       </c>
@@ -9397,15 +9755,17 @@
         <v>179</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>859</v>
+        <v>851</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>1003</v>
-      </c>
-      <c r="E181" s="2"/>
+        <v>994</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>1041</v>
+      </c>
       <c r="F181" s="1">
         <v>4</v>
       </c>
@@ -9429,7 +9789,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>860</v>
+        <v>852</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>773</v>
@@ -9481,7 +9841,7 @@
         <v>788</v>
       </c>
       <c r="K183" s="1" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
     </row>
     <row r="184" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -9539,7 +9899,7 @@
         <v>788</v>
       </c>
       <c r="K185" s="1" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
     </row>
     <row r="186" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -9597,7 +9957,7 @@
         <v>788</v>
       </c>
       <c r="K187" s="1" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.3">
@@ -9605,7 +9965,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>773</v>
@@ -9631,7 +9991,7 @@
         <v>787</v>
       </c>
       <c r="K188" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.3">
@@ -9639,7 +9999,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>773</v>
@@ -9665,7 +10025,7 @@
         <v>787</v>
       </c>
       <c r="K189" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.3">
@@ -9673,7 +10033,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>773</v>
@@ -9699,7 +10059,7 @@
         <v>787</v>
       </c>
       <c r="K190" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.3">
@@ -9707,7 +10067,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>773</v>
@@ -9733,7 +10093,7 @@
         <v>787</v>
       </c>
       <c r="K191" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.3">
@@ -9741,7 +10101,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>773</v>
@@ -9767,7 +10127,7 @@
         <v>787</v>
       </c>
       <c r="K192" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.3">
@@ -9775,7 +10135,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>773</v>
@@ -9801,7 +10161,7 @@
         <v>787</v>
       </c>
       <c r="K193" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.3">
@@ -9809,7 +10169,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>773</v>
@@ -9835,7 +10195,7 @@
         <v>787</v>
       </c>
       <c r="K194" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.3">
@@ -9843,7 +10203,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>773</v>
@@ -9869,7 +10229,7 @@
         <v>787</v>
       </c>
       <c r="K195" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.3">
@@ -9877,7 +10237,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>773</v>
@@ -9903,7 +10263,7 @@
         <v>787</v>
       </c>
       <c r="K196" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.3">
@@ -9911,7 +10271,7 @@
         <v>195</v>
       </c>
       <c r="B197" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>773</v>
@@ -9937,7 +10297,7 @@
         <v>787</v>
       </c>
       <c r="K197" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.3">
@@ -9945,7 +10305,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>773</v>
@@ -9971,7 +10331,7 @@
         <v>787</v>
       </c>
       <c r="K198" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.3">
@@ -9979,7 +10339,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>773</v>
@@ -10005,7 +10365,7 @@
         <v>787</v>
       </c>
       <c r="K199" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.3">
@@ -10013,7 +10373,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>773</v>
@@ -10039,7 +10399,7 @@
         <v>787</v>
       </c>
       <c r="K200" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.3">
@@ -10047,7 +10407,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>773</v>
@@ -10073,7 +10433,7 @@
         <v>787</v>
       </c>
       <c r="K201" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.3">
@@ -10081,7 +10441,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>773</v>
@@ -10107,7 +10467,7 @@
         <v>787</v>
       </c>
       <c r="K202" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.3">
@@ -10115,7 +10475,7 @@
         <v>201</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>773</v>
@@ -10141,7 +10501,7 @@
         <v>787</v>
       </c>
       <c r="K203" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.3">
@@ -10149,7 +10509,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>773</v>
@@ -10175,7 +10535,7 @@
         <v>787</v>
       </c>
       <c r="K204" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.3">
@@ -10183,7 +10543,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>773</v>
@@ -10209,7 +10569,7 @@
         <v>787</v>
       </c>
       <c r="K205" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
@@ -10217,7 +10577,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>773</v>
@@ -10243,7 +10603,7 @@
         <v>787</v>
       </c>
       <c r="K206" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.3">
@@ -10251,7 +10611,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>773</v>
@@ -10277,7 +10637,7 @@
         <v>787</v>
       </c>
       <c r="K207" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.3">
@@ -10285,7 +10645,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>773</v>
@@ -10311,7 +10671,7 @@
         <v>787</v>
       </c>
       <c r="K208" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.3">
@@ -10319,7 +10679,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>773</v>
@@ -10345,7 +10705,7 @@
         <v>787</v>
       </c>
       <c r="K209" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.3">
@@ -10353,7 +10713,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>773</v>
@@ -10379,7 +10739,7 @@
         <v>787</v>
       </c>
       <c r="K210" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.3">
@@ -10387,7 +10747,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>773</v>
@@ -10413,7 +10773,7 @@
         <v>787</v>
       </c>
       <c r="K211" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.3">
@@ -10421,7 +10781,7 @@
         <v>210</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>773</v>
@@ -10447,7 +10807,7 @@
         <v>787</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.3">
@@ -10455,7 +10815,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>773</v>
@@ -10481,7 +10841,7 @@
         <v>787</v>
       </c>
       <c r="K213" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.3">
@@ -10489,7 +10849,7 @@
         <v>212</v>
       </c>
       <c r="B214" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>773</v>
@@ -10515,7 +10875,7 @@
         <v>787</v>
       </c>
       <c r="K214" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.3">
@@ -10523,7 +10883,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>773</v>
@@ -10549,7 +10909,7 @@
         <v>787</v>
       </c>
       <c r="K215" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.3">
@@ -10557,7 +10917,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>773</v>
@@ -10583,7 +10943,7 @@
         <v>787</v>
       </c>
       <c r="K216" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.3">
@@ -10591,7 +10951,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>773</v>
@@ -10617,7 +10977,7 @@
         <v>787</v>
       </c>
       <c r="K217" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.3">
@@ -10625,7 +10985,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>773</v>
@@ -10651,7 +11011,7 @@
         <v>787</v>
       </c>
       <c r="K218" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.3">
@@ -10659,7 +11019,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>773</v>
@@ -10685,7 +11045,7 @@
         <v>787</v>
       </c>
       <c r="K219" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.3">
@@ -10693,7 +11053,7 @@
         <v>218</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>773</v>
@@ -10719,7 +11079,7 @@
         <v>787</v>
       </c>
       <c r="K220" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.3">
@@ -10727,7 +11087,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>773</v>
@@ -10753,7 +11113,7 @@
         <v>787</v>
       </c>
       <c r="K221" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.3">
@@ -10761,7 +11121,7 @@
         <v>220</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>773</v>
@@ -10787,7 +11147,7 @@
         <v>787</v>
       </c>
       <c r="K222" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.3">
@@ -10795,7 +11155,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>773</v>
@@ -10821,7 +11181,7 @@
         <v>787</v>
       </c>
       <c r="K223" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.3">
@@ -10829,7 +11189,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>773</v>
@@ -10855,7 +11215,7 @@
         <v>787</v>
       </c>
       <c r="K224" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.3">
@@ -10863,7 +11223,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>773</v>
@@ -10889,7 +11249,7 @@
         <v>787</v>
       </c>
       <c r="K225" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.3">
@@ -10897,7 +11257,7 @@
         <v>224</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C226" s="2" t="s">
         <v>773</v>
@@ -10923,7 +11283,7 @@
         <v>787</v>
       </c>
       <c r="K226" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.3">
@@ -10931,7 +11291,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>773</v>
@@ -10957,7 +11317,7 @@
         <v>787</v>
       </c>
       <c r="K227" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.3">
@@ -10965,7 +11325,7 @@
         <v>226</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>773</v>
@@ -10991,7 +11351,7 @@
         <v>787</v>
       </c>
       <c r="K228" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.3">
@@ -10999,7 +11359,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>773</v>
@@ -11025,7 +11385,7 @@
         <v>787</v>
       </c>
       <c r="K229" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.3">
@@ -11033,7 +11393,7 @@
         <v>228</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>773</v>
@@ -11059,7 +11419,7 @@
         <v>787</v>
       </c>
       <c r="K230" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.3">
@@ -11067,7 +11427,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>773</v>
@@ -11093,7 +11453,7 @@
         <v>787</v>
       </c>
       <c r="K231" s="1" t="s">
-        <v>999</v>
+        <v>990</v>
       </c>
     </row>
     <row r="232" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11381,15 +11741,17 @@
         <v>240</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>1002</v>
-      </c>
-      <c r="E242" s="2"/>
+        <v>993</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>1042</v>
+      </c>
       <c r="F242" s="1">
         <v>855</v>
       </c>
@@ -11413,15 +11775,17 @@
         <v>241</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>1004</v>
-      </c>
-      <c r="E243" s="2"/>
+        <v>995</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>1043</v>
+      </c>
       <c r="F243" s="1">
         <v>17</v>
       </c>
@@ -11445,7 +11809,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>774</v>
@@ -11453,7 +11817,9 @@
       <c r="D244" s="2" t="s">
         <v>821</v>
       </c>
-      <c r="E244" s="2"/>
+      <c r="E244" s="2" t="s">
+        <v>1027</v>
+      </c>
       <c r="F244" s="1">
         <v>5</v>
       </c>
@@ -11477,7 +11843,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>774</v>
@@ -11485,7 +11851,9 @@
       <c r="D245" s="2" t="s">
         <v>821</v>
       </c>
-      <c r="E245" s="2"/>
+      <c r="E245" s="2" t="s">
+        <v>1044</v>
+      </c>
       <c r="F245" s="1">
         <v>14</v>
       </c>
@@ -11509,7 +11877,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>773</v>
@@ -13211,7 +13579,7 @@
         <v>301</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>773</v>
@@ -13241,7 +13609,7 @@
         <v>302</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>773</v>
@@ -13271,7 +13639,7 @@
         <v>303</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>773</v>
@@ -13301,7 +13669,7 @@
         <v>304</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>774</v>
@@ -13325,7 +13693,7 @@
         <v>788</v>
       </c>
       <c r="K306" s="1" t="s">
-        <v>964</v>
+        <v>956</v>
       </c>
     </row>
     <row r="307" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13333,7 +13701,7 @@
         <v>305</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>773</v>
@@ -13363,7 +13731,7 @@
         <v>306</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>966</v>
+        <v>958</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>773</v>
@@ -13393,7 +13761,7 @@
         <v>307</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>967</v>
+        <v>959</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>773</v>
@@ -13423,7 +13791,7 @@
         <v>308</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>774</v>
@@ -13447,7 +13815,7 @@
         <v>788</v>
       </c>
       <c r="K310" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="311" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -13455,7 +13823,7 @@
         <v>309</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>969</v>
+        <v>961</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>773</v>
@@ -13485,7 +13853,7 @@
         <v>310</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>773</v>
@@ -13515,7 +13883,7 @@
         <v>311</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>971</v>
+        <v>963</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>773</v>
@@ -13545,7 +13913,7 @@
         <v>312</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>972</v>
+        <v>964</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>773</v>
@@ -13575,7 +13943,7 @@
         <v>313</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>973</v>
+        <v>965</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>773</v>
@@ -13605,7 +13973,7 @@
         <v>314</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>974</v>
+        <v>966</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>773</v>
@@ -13635,7 +14003,7 @@
         <v>315</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>975</v>
+        <v>967</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>773</v>
@@ -13665,7 +14033,7 @@
         <v>316</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>976</v>
+        <v>968</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>773</v>
@@ -13695,13 +14063,15 @@
         <v>317</v>
       </c>
       <c r="B319" s="1" t="s">
-        <v>977</v>
+        <v>969</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D319" s="2"/>
-      <c r="E319" s="2"/>
+      <c r="E319" s="2" t="s">
+        <v>1045</v>
+      </c>
       <c r="F319" s="1">
         <v>3</v>
       </c>
@@ -16889,7 +17259,7 @@
         <v>431</v>
       </c>
       <c r="B433" s="1" t="s">
-        <v>979</v>
+        <v>971</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>774</v>
@@ -16910,9 +17280,11 @@
         <v>0</v>
       </c>
       <c r="J433" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="K433" s="1"/>
+        <v>788</v>
+      </c>
+      <c r="K433" s="1" t="s">
+        <v>1006</v>
+      </c>
     </row>
     <row r="434" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" s="1" t="s">
@@ -18771,7 +19143,7 @@
         <v>498</v>
       </c>
       <c r="B500" s="1" t="s">
-        <v>980</v>
+        <v>972</v>
       </c>
       <c r="C500" s="2" t="s">
         <v>775</v>
@@ -18795,7 +19167,7 @@
         <v>788</v>
       </c>
       <c r="K500" s="1" t="s">
-        <v>981</v>
+        <v>973</v>
       </c>
     </row>
     <row r="501" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -18803,7 +19175,7 @@
         <v>499</v>
       </c>
       <c r="B501" s="1" t="s">
-        <v>982</v>
+        <v>974</v>
       </c>
       <c r="C501" s="2" t="s">
         <v>773</v>
@@ -18827,7 +19199,7 @@
         <v>788</v>
       </c>
       <c r="K501" s="1" t="s">
-        <v>983</v>
+        <v>975</v>
       </c>
     </row>
     <row r="502" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -18835,7 +19207,7 @@
         <v>500</v>
       </c>
       <c r="B502" s="1" t="s">
-        <v>984</v>
+        <v>976</v>
       </c>
       <c r="C502" s="2" t="s">
         <v>775</v>
@@ -18859,7 +19231,7 @@
         <v>788</v>
       </c>
       <c r="K502" s="1" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
     </row>
     <row r="503" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -18867,7 +19239,7 @@
         <v>501</v>
       </c>
       <c r="B503" s="1" t="s">
-        <v>986</v>
+        <v>978</v>
       </c>
       <c r="C503" s="2" t="s">
         <v>775</v>
@@ -18891,7 +19263,7 @@
         <v>788</v>
       </c>
       <c r="K503" s="1" t="s">
-        <v>987</v>
+        <v>979</v>
       </c>
     </row>
     <row r="504" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20069,7 +20441,7 @@
         <v>788</v>
       </c>
       <c r="K545" s="1" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
     </row>
     <row r="546" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20099,7 +20471,7 @@
         <v>788</v>
       </c>
       <c r="K546" s="1" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
     </row>
     <row r="547" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20129,7 +20501,7 @@
         <v>788</v>
       </c>
       <c r="K547" s="1" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
     </row>
     <row r="548" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20159,7 +20531,7 @@
         <v>788</v>
       </c>
       <c r="K548" s="1" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
     </row>
     <row r="549" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -20189,7 +20561,7 @@
         <v>788</v>
       </c>
       <c r="K549" s="1" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
     </row>
     <row r="550" spans="1:11" x14ac:dyDescent="0.3">
@@ -20197,7 +20569,7 @@
         <v>548</v>
       </c>
       <c r="B550" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C550" s="2" t="s">
         <v>773</v>
@@ -20227,7 +20599,7 @@
         <v>549</v>
       </c>
       <c r="B551" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C551" s="2" t="s">
         <v>773</v>
@@ -20257,7 +20629,7 @@
         <v>550</v>
       </c>
       <c r="B552" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C552" s="2" t="s">
         <v>773</v>
@@ -20287,7 +20659,7 @@
         <v>551</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C553" s="2" t="s">
         <v>773</v>
@@ -21773,7 +22145,7 @@
         <v>604</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="C606" s="2" t="s">
         <v>773</v>
@@ -21803,7 +22175,7 @@
         <v>605</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="C607" s="2" t="s">
         <v>773</v>
@@ -22335,7 +22707,7 @@
         <v>788</v>
       </c>
       <c r="K625" s="1" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
     </row>
     <row r="626" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -23513,7 +23885,7 @@
         <v>788</v>
       </c>
       <c r="K667" s="1" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
     </row>
     <row r="668" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25087,7 +25459,7 @@
         <v>788</v>
       </c>
       <c r="K723" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="724" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25117,7 +25489,7 @@
         <v>788</v>
       </c>
       <c r="K724" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="725" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25147,7 +25519,7 @@
         <v>788</v>
       </c>
       <c r="K725" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="726" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25177,7 +25549,7 @@
         <v>788</v>
       </c>
       <c r="K726" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="727" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25207,7 +25579,7 @@
         <v>788</v>
       </c>
       <c r="K727" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="728" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25237,7 +25609,7 @@
         <v>788</v>
       </c>
       <c r="K728" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="729" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25267,7 +25639,7 @@
         <v>788</v>
       </c>
       <c r="K729" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="730" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25297,7 +25669,7 @@
         <v>788</v>
       </c>
       <c r="K730" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="731" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25327,7 +25699,7 @@
         <v>788</v>
       </c>
       <c r="K731" s="1" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
     </row>
     <row r="732" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25335,13 +25707,15 @@
         <v>730</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>995</v>
+        <v>1046</v>
       </c>
       <c r="C732" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D732" s="2"/>
-      <c r="E732" s="2"/>
+      <c r="E732" s="2" t="s">
+        <v>1047</v>
+      </c>
       <c r="F732" s="1">
         <v>4</v>
       </c>
@@ -25365,7 +25739,7 @@
         <v>731</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>1005</v>
+        <v>996</v>
       </c>
       <c r="C733" s="2" t="s">
         <v>773</v>
@@ -25397,7 +25771,7 @@
         <v>732</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="C734" s="2" t="s">
         <v>775</v>
@@ -25421,7 +25795,7 @@
         <v>788</v>
       </c>
       <c r="K734" s="1" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
     </row>
     <row r="735" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25429,15 +25803,17 @@
         <v>733</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>1006</v>
+        <v>997</v>
       </c>
       <c r="C735" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D735" s="2" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E735" s="2"/>
+        <v>992</v>
+      </c>
+      <c r="E735" s="2" t="s">
+        <v>1049</v>
+      </c>
       <c r="F735" s="1">
         <v>6</v>
       </c>
@@ -25483,7 +25859,7 @@
         <v>788</v>
       </c>
       <c r="K736" s="1" t="s">
-        <v>996</v>
+        <v>987</v>
       </c>
     </row>
     <row r="737" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -25491,7 +25867,7 @@
         <v>735</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>1007</v>
+        <v>998</v>
       </c>
       <c r="C737" s="2" t="s">
         <v>773</v>
@@ -25522,12 +25898,16 @@
       <c r="A738" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="B738" s="1"/>
+      <c r="B738" s="1" t="s">
+        <v>1048</v>
+      </c>
       <c r="C738" s="2" t="s">
         <v>774</v>
       </c>
       <c r="D738" s="2"/>
-      <c r="E738" s="2"/>
+      <c r="E738" s="2" t="s">
+        <v>1047</v>
+      </c>
       <c r="F738" s="1">
         <v>4</v>
       </c>
@@ -25719,7 +26099,7 @@
         <v>743</v>
       </c>
       <c r="B745" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C745" s="2" t="s">
         <v>773</v>
@@ -25749,7 +26129,7 @@
         <v>744</v>
       </c>
       <c r="B746" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C746" s="2" t="s">
         <v>773</v>
@@ -26087,7 +26467,7 @@
         <v>756</v>
       </c>
       <c r="B758" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C758" s="2" t="s">
         <v>773</v>
@@ -26119,7 +26499,7 @@
         <v>757</v>
       </c>
       <c r="B759" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C759" s="2" t="s">
         <v>773</v>
@@ -26151,7 +26531,7 @@
         <v>758</v>
       </c>
       <c r="B760" s="4" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="C760" s="2" t="s">
         <v>773</v>
@@ -26379,7 +26759,7 @@
         <v>766</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="C768" s="2" t="s">
         <v>773</v>
@@ -26403,7 +26783,7 @@
         <v>788</v>
       </c>
       <c r="K768" s="1" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>